<commit_message>
Work Item 5 Update.
Fix pop up automation issue.
</commit_message>
<xml_diff>
--- a/SourceCode/2023/Sep2023/Projects/Yannick/ACME_Work_Item_5/Data/Config.xlsx
+++ b/SourceCode/2023/Sep2023/Projects/Yannick/ACME_Work_Item_5/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannick\Documents\UiPath\Training\UiARD\ACME_Work_Item_5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannick\Documents\RPA\Uipath\GitHub\RPA-Developer-in-30-Days\SourceCode\2023\Sep2023\Projects\Yannick\ACME_Work_Item_5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C88A30-8A00-4992-8E52-BDB52E3CE15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E689F2-E29A-4E03-9F6D-2278B05EB1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="13695" yWindow="4575" windowWidth="20205" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2610" yWindow="2805" windowWidth="10103" windowHeight="5490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>UpdateItemUrl</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/update/</t>
   </si>
 </sst>
 </file>
@@ -213,18 +219,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,13 +462,13 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -554,7 +563,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1547,6 +1563,7 @@
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{AAF851D9-3512-4300-BE5B-0E135CBAEEB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>